<commit_message>
Add support for briefing participants import and display
Implemented functionality to import and display briefing (説明会) participants from CSV/Excel files. Updated the UI to allow separate file input for briefing participants, display their list grouped by time, and synchronize attendance status. Added new styles for the briefing participant section and updated sample files.
</commit_message>
<xml_diff>
--- a/Reception/sample_cs_preferences_30.xlsx
+++ b/Reception/sample_cs_preferences_30.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deer/Prog/SHICA_LANG/OpenCampus/Reception/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533A2824-CC1D-E842-BEAF-41455089C8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="880" windowWidth="27040" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -472,12 +478,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -485,8 +491,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -532,17 +545,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -580,7 +601,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -614,6 +635,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -648,9 +670,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -823,12 +846,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="15" max="15" width="54" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
@@ -2438,6 +2466,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>